<commit_message>
Add new power plants to Electricity Source subscript (issues #280 and #99)
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
+++ b/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\bldgs\SYDEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71857E9-CBEA-41F2-BB27-BB1134E561B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312F2049-2A06-44C6-A79C-EBBBFE07E60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="553">
   <si>
     <t>Energy Information Administration</t>
   </si>
@@ -1846,6 +1846,24 @@
   </si>
   <si>
     <t>natural gas combined cycle</t>
+  </si>
+  <si>
+    <t>hard coal w CCS</t>
+  </si>
+  <si>
+    <t>natural gas combined cycle w CCS</t>
+  </si>
+  <si>
+    <t>biomass w CCS</t>
+  </si>
+  <si>
+    <t>lignite w CCS</t>
+  </si>
+  <si>
+    <t>small modular reactor</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
   </si>
 </sst>
 </file>
@@ -14512,9 +14530,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -14552,9 +14570,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -14587,26 +14605,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -14639,26 +14640,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -34274,10 +34258,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D3"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34547,6 +34531,90 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>547</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>548</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>549</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>550</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>551</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>552</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add hydrogen combined cycle as a power plant type (#99)
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
+++ b/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\bldgs\SYDEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312F2049-2A06-44C6-A79C-EBBBFE07E60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F68715-1BDC-4F96-B4F9-DAECB448B85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="554">
   <si>
     <t>Energy Information Administration</t>
   </si>
@@ -1863,7 +1863,10 @@
     <t>small modular reactor</t>
   </si>
   <si>
-    <t>hydrogen</t>
+    <t>hydrogen combustion turbine</t>
+  </si>
+  <si>
+    <t>hydrogen combined cycle</t>
   </si>
 </sst>
 </file>
@@ -1874,7 +1877,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1990,6 +1993,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2172,7 +2182,7 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2262,6 +2272,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="10">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -34258,10 +34271,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B25" sqref="B25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34602,7 +34615,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="36" t="s">
         <v>552</v>
       </c>
       <c r="B24">
@@ -34612,6 +34625,20 @@
         <v>0</v>
       </c>
       <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>553</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
         <v>0</v>
       </c>
     </row>

</xml_diff>